<commit_message>
ITC-XX - Add Mutual Loan Credit XSD schema and adjust `MutualLoanCreditExportXML` field handling: include `mutualLoanCredit.xsd`, fix `clave_actividad` text value to `MPC`, and improve priority element handling logic.
</commit_message>
<xml_diff>
--- a/public/templates/plantillaMutuoPrestamoCredito.xlsx
+++ b/public/templates/plantillaMutuoPrestamoCredito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrrme\Downloads\PLD\Mutuo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EA76B3-D9A8-46FE-B591-82B5060E0B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC60851F-2B61-4ADF-8DA7-EADC71E5C111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="1011">
   <si>
     <t>Forma de pago</t>
   </si>
@@ -3083,6 +3083,15 @@
   </si>
   <si>
     <t>Alerta</t>
+  </si>
+  <si>
+    <t>Priodidad</t>
+  </si>
+  <si>
+    <t>1 - Normal</t>
+  </si>
+  <si>
+    <t>2 - 24 Hrs. con operaciones</t>
   </si>
 </sst>
 </file>
@@ -3197,7 +3206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -3395,13 +3404,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3446,7 +3466,19 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3455,24 +3487,16 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -5549,12 +5573,15 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:CD104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BT1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BN6" sqref="BN6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
@@ -5624,71 +5651,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:82" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>966</v>
       </c>
       <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="27" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="24" t="s">
         <v>1007</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="25" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="29" t="s">
         <v>950</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="25"/>
-      <c r="AO1" s="25"/>
-      <c r="AP1" s="25"/>
-      <c r="AQ1" s="25"/>
-      <c r="AR1" s="28" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="29"/>
+      <c r="AR1" s="31" t="s">
         <v>951</v>
       </c>
-      <c r="AS1" s="28"/>
-      <c r="AT1" s="28"/>
-      <c r="AU1" s="28"/>
-      <c r="AV1" s="28"/>
-      <c r="AW1" s="28"/>
-      <c r="AX1" s="28"/>
-      <c r="AY1" s="28"/>
-      <c r="AZ1" s="28"/>
-      <c r="BA1" s="28"/>
-      <c r="BB1" s="28"/>
-      <c r="BC1" s="28"/>
-      <c r="BD1" s="28"/>
-      <c r="BE1" s="28"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
+      <c r="AW1" s="31"/>
+      <c r="AX1" s="31"/>
+      <c r="AY1" s="31"/>
+      <c r="AZ1" s="31"/>
+      <c r="BA1" s="31"/>
+      <c r="BB1" s="31"/>
+      <c r="BC1" s="31"/>
+      <c r="BD1" s="31"/>
+      <c r="BE1" s="31"/>
       <c r="BF1" s="21" t="s">
         <v>954</v>
       </c>
@@ -5700,14 +5727,14 @@
       <c r="BL1" s="22"/>
       <c r="BM1" s="22"/>
       <c r="BN1" s="22"/>
-      <c r="BO1" s="24" t="s">
+      <c r="BO1" s="27" t="s">
         <v>983</v>
       </c>
-      <c r="BP1" s="24"/>
-      <c r="BQ1" s="24"/>
-      <c r="BR1" s="24"/>
-      <c r="BS1" s="24"/>
-      <c r="BT1" s="24"/>
+      <c r="BP1" s="27"/>
+      <c r="BQ1" s="27"/>
+      <c r="BR1" s="27"/>
+      <c r="BS1" s="27"/>
+      <c r="BT1" s="27"/>
       <c r="BU1" s="15"/>
       <c r="BV1" s="15"/>
       <c r="BW1" s="15"/>
@@ -5720,126 +5747,126 @@
       <c r="CD1" s="23"/>
     </row>
     <row r="2" spans="1:82" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>967</v>
       </c>
       <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="27" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="24" t="s">
         <v>1007</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="25" t="s">
+      <c r="E2" s="25"/>
+      <c r="F2" s="29" t="s">
         <v>935</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29" t="s">
         <v>940</v>
       </c>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25" t="s">
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29" t="s">
         <v>912</v>
       </c>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="31" t="s">
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="32" t="s">
         <v>944</v>
       </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="25" t="s">
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="29" t="s">
         <v>914</v>
       </c>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25"/>
-      <c r="AE2" s="25"/>
-      <c r="AF2" s="25"/>
-      <c r="AG2" s="25" t="s">
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29" t="s">
         <v>921</v>
       </c>
-      <c r="AH2" s="25"/>
-      <c r="AI2" s="25"/>
-      <c r="AJ2" s="25"/>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25" t="s">
+      <c r="AH2" s="29"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29"/>
+      <c r="AO2" s="29" t="s">
         <v>980</v>
       </c>
-      <c r="AP2" s="25"/>
-      <c r="AQ2" s="25"/>
-      <c r="AR2" s="25" t="s">
+      <c r="AP2" s="29"/>
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="29" t="s">
         <v>909</v>
       </c>
-      <c r="AS2" s="25"/>
-      <c r="AT2" s="25"/>
-      <c r="AU2" s="25"/>
-      <c r="AV2" s="25"/>
-      <c r="AW2" s="25"/>
-      <c r="AX2" s="25"/>
-      <c r="AY2" s="25" t="s">
+      <c r="AS2" s="29"/>
+      <c r="AT2" s="29"/>
+      <c r="AU2" s="29"/>
+      <c r="AV2" s="29"/>
+      <c r="AW2" s="29"/>
+      <c r="AX2" s="29"/>
+      <c r="AY2" s="29" t="s">
         <v>911</v>
       </c>
-      <c r="AZ2" s="25"/>
-      <c r="BA2" s="25"/>
-      <c r="BB2" s="25"/>
-      <c r="BC2" s="25" t="s">
+      <c r="AZ2" s="29"/>
+      <c r="BA2" s="29"/>
+      <c r="BB2" s="29"/>
+      <c r="BC2" s="29" t="s">
         <v>912</v>
       </c>
-      <c r="BD2" s="25"/>
-      <c r="BE2" s="27"/>
-      <c r="BF2" s="29" t="s">
+      <c r="BD2" s="29"/>
+      <c r="BE2" s="24"/>
+      <c r="BF2" s="26" t="s">
         <v>955</v>
       </c>
-      <c r="BG2" s="24"/>
-      <c r="BH2" s="24"/>
-      <c r="BI2" s="24"/>
-      <c r="BJ2" s="29" t="s">
+      <c r="BG2" s="27"/>
+      <c r="BH2" s="27"/>
+      <c r="BI2" s="27"/>
+      <c r="BJ2" s="26" t="s">
         <v>978</v>
       </c>
-      <c r="BK2" s="24"/>
-      <c r="BL2" s="24"/>
-      <c r="BM2" s="30"/>
+      <c r="BK2" s="27"/>
+      <c r="BL2" s="27"/>
+      <c r="BM2" s="28"/>
       <c r="BN2" s="16" t="s">
         <v>979</v>
       </c>
-      <c r="BO2" s="29" t="s">
+      <c r="BO2" s="26" t="s">
         <v>982</v>
       </c>
-      <c r="BP2" s="24"/>
-      <c r="BQ2" s="24"/>
-      <c r="BR2" s="24"/>
-      <c r="BS2" s="24"/>
-      <c r="BT2" s="30"/>
-      <c r="BU2" s="29" t="s">
+      <c r="BP2" s="27"/>
+      <c r="BQ2" s="27"/>
+      <c r="BR2" s="27"/>
+      <c r="BS2" s="27"/>
+      <c r="BT2" s="28"/>
+      <c r="BU2" s="26" t="s">
         <v>984</v>
       </c>
-      <c r="BV2" s="24"/>
-      <c r="BW2" s="30"/>
-      <c r="BX2" s="29" t="s">
+      <c r="BV2" s="27"/>
+      <c r="BW2" s="28"/>
+      <c r="BX2" s="26" t="s">
         <v>912</v>
       </c>
-      <c r="BY2" s="24"/>
-      <c r="BZ2" s="30"/>
-      <c r="CA2" s="26" t="s">
+      <c r="BY2" s="27"/>
+      <c r="BZ2" s="28"/>
+      <c r="CA2" s="30" t="s">
         <v>957</v>
       </c>
-      <c r="CB2" s="26"/>
-      <c r="CC2" s="26"/>
-      <c r="CD2" s="26"/>
+      <c r="CB2" s="30"/>
+      <c r="CC2" s="30"/>
+      <c r="CD2" s="30"/>
     </row>
     <row r="3" spans="1:82" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
@@ -15180,17 +15207,9 @@
     </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" insertHyperlinks="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <dataConsolidate/>
   <mergeCells count="23">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="BU2:BW2"/>
-    <mergeCell ref="BX2:BZ2"/>
-    <mergeCell ref="AG2:AN2"/>
-    <mergeCell ref="BF2:BI2"/>
-    <mergeCell ref="BO2:BT2"/>
-    <mergeCell ref="BO1:BT1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A2:B2"/>
     <mergeCell ref="CA2:CD2"/>
     <mergeCell ref="AO2:AQ2"/>
     <mergeCell ref="BC2:BE2"/>
@@ -15204,8 +15223,17 @@
     <mergeCell ref="V2:AA2"/>
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="AB2:AF2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="BU2:BW2"/>
+    <mergeCell ref="BX2:BZ2"/>
+    <mergeCell ref="AG2:AN2"/>
+    <mergeCell ref="BF2:BI2"/>
+    <mergeCell ref="BO2:BT2"/>
+    <mergeCell ref="BO1:BT1"/>
   </mergeCells>
-  <dataValidations xWindow="491" yWindow="317" count="24">
+  <dataValidations xWindow="491" yWindow="317" count="25">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de llenado" error="No debe de contener espacios ni caracteres especiales." promptTitle="Indicaciones" prompt="El formato debe ser XAXX010101000." sqref="J4:J104 Z4:Z104 AV4:AV104" xr:uid="{B98F17B9-63D0-482A-929E-F8CFD205118A}">
       <formula1>0</formula1>
       <formula2>13</formula2>
@@ -15223,7 +15251,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de llenado" error="Seleccionar un giro mercantil de la lista desplegable." promptTitle="Indicaciones" prompt="Seleccionar un giro mercantil de la lista desplegable." sqref="R4:R104" xr:uid="{27088C97-E5CF-4F9B-9C69-044AD9E3433B}">
       <formula1>giro</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de llenado" error="El campo debe contener máximo 200 dígitos." sqref="AR4:AT104 V4:X104 A4:C104 E4:H104" xr:uid="{28F6DE79-B026-4485-A4B3-B8E797F9725E}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de llenado" error="El campo debe contener máximo 200 dígitos." sqref="AR4:AT104 V4:X104 E4:H104 A4:B104" xr:uid="{28F6DE79-B026-4485-A4B3-B8E797F9725E}">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
@@ -15286,17 +15314,20 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de llenado" error="Se debe de seleccionar una moneda de la lista desplegable." promptTitle="Indicaciones" prompt="Seleccionar una moneda de la desplegable." sqref="CC5:CC104" xr:uid="{B99C83B5-C1D0-47C8-9C66-BC56244D232A}">
       <formula1>moneda</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="BM5:BZ104 BM4:CC4" xr:uid="{0EB29509-B241-424B-A450-CE8133913FB3}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="BM5:BZ104 BM4:CA4" xr:uid="{0EB29509-B241-424B-A450-CE8133913FB3}"/>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de llenado" error="Ingresar mínimo 4 dígitos o máximo 17 dígitos. _x000a_Es obligatorio que se especifiquen los decimales, aún cuando la cantidad fraccionaria sea .00" promptTitle="Indicaciones" prompt="Ingresar mínimo 4 dígitos o máximo 17 dígitos. _x000a_Es obligatorio que se especifiquen los decimales, aún cuando la cantidad fraccionaria sea .00" sqref="CD5:CD104" xr:uid="{016B7E29-830C-46F9-AF25-446454427453}">
       <formula1>1111</formula1>
       <formula2>99999999999999900</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="CC4" xr:uid="{C7FC1AF3-3535-402B-8888-A1E9F0F5932A}">
+      <formula1>moneda</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="491" yWindow="317" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="491" yWindow="317" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de llenado" error="El campo no debe contener espacios, caracteres especiales ni letras y únicamente debe contener dígitos." promptTitle="Indicaciones" prompt="El formato debe ser AAAAMMDD." xr:uid="{7D440FE5-DD57-494F-BB11-C91C0C71E5BB}">
           <x14:formula1>
             <xm:f>Configuracion!$AS$3:$AS$4</xm:f>
@@ -15321,6 +15352,18 @@
           </x14:formula1>
           <xm:sqref>D3:D104</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de llenado" error="El campo debe contener máximo 200 dígitos." xr:uid="{2FD3809B-0D16-477F-821D-5CFC70F48194}">
+          <x14:formula1>
+            <xm:f>Configuracion!$E$3:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4:C104</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{94E66A33-3E50-4A82-BAFC-01B1FC5353FB}">
+          <x14:formula1>
+            <xm:f>Configuracion!$Q$3:$Q$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>CB4</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -15332,14 +15375,15 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A2:AU251"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="F152" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" customWidth="1"/>
   </cols>
@@ -15357,6 +15401,9 @@
       <c r="D2" s="1" t="s">
         <v>922</v>
       </c>
+      <c r="E2" s="33" t="s">
+        <v>1008</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
@@ -15434,6 +15481,9 @@
       <c r="D3" t="s">
         <v>923</v>
       </c>
+      <c r="E3" t="s">
+        <v>1009</v>
+      </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
@@ -15507,6 +15557,9 @@
       </c>
       <c r="D4" t="s">
         <v>924</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1010</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
ITC-XX - Update login page logo and replace plantillaMutuoPrestamoCredito template.
</commit_message>
<xml_diff>
--- a/public/templates/plantillaMutuoPrestamoCredito.xlsx
+++ b/public/templates/plantillaMutuoPrestamoCredito.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrrme\Downloads\PLD\Mutuo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\jrrmelecio\projects\itc-pld\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC60851F-2B61-4ADF-8DA7-EADC71E5C111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA53E8C-FC87-426B-8FAA-9741A4CCE562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="9" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="1011">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="1011">
   <si>
     <t>Forma de pago</t>
   </si>
@@ -3466,10 +3466,23 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3482,21 +3495,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -5573,8 +5573,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:CD104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BT1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BN6" sqref="BN6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5651,15 +5651,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:82" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>966</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="24" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="25" t="s">
+        <v>970</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>1007</v>
       </c>
-      <c r="E1" s="25"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="29" t="s">
         <v>950</v>
       </c>
@@ -5700,22 +5702,22 @@
       <c r="AO1" s="29"/>
       <c r="AP1" s="29"/>
       <c r="AQ1" s="29"/>
-      <c r="AR1" s="31" t="s">
+      <c r="AR1" s="30" t="s">
         <v>951</v>
       </c>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="30"/>
+      <c r="AW1" s="30"/>
+      <c r="AX1" s="30"/>
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="30"/>
       <c r="BF1" s="21" t="s">
         <v>954</v>
       </c>
@@ -5727,14 +5729,14 @@
       <c r="BL1" s="22"/>
       <c r="BM1" s="22"/>
       <c r="BN1" s="22"/>
-      <c r="BO1" s="27" t="s">
+      <c r="BO1" s="32" t="s">
         <v>983</v>
       </c>
-      <c r="BP1" s="27"/>
-      <c r="BQ1" s="27"/>
-      <c r="BR1" s="27"/>
-      <c r="BS1" s="27"/>
-      <c r="BT1" s="27"/>
+      <c r="BP1" s="32"/>
+      <c r="BQ1" s="32"/>
+      <c r="BR1" s="32"/>
+      <c r="BS1" s="32"/>
+      <c r="BT1" s="32"/>
       <c r="BU1" s="15"/>
       <c r="BV1" s="15"/>
       <c r="BW1" s="15"/>
@@ -5747,15 +5749,17 @@
       <c r="CD1" s="23"/>
     </row>
     <row r="2" spans="1:82" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="26" t="s">
         <v>967</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="24" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="25" t="s">
+        <v>970</v>
+      </c>
+      <c r="D2" s="26" t="s">
         <v>1007</v>
       </c>
-      <c r="E2" s="25"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="29" t="s">
         <v>935</v>
       </c>
@@ -5778,14 +5782,14 @@
       </c>
       <c r="T2" s="29"/>
       <c r="U2" s="29"/>
-      <c r="V2" s="32" t="s">
+      <c r="V2" s="34" t="s">
         <v>944</v>
       </c>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="34"/>
       <c r="AB2" s="29" t="s">
         <v>914</v>
       </c>
@@ -5827,46 +5831,46 @@
         <v>912</v>
       </c>
       <c r="BD2" s="29"/>
-      <c r="BE2" s="24"/>
-      <c r="BF2" s="26" t="s">
+      <c r="BE2" s="26"/>
+      <c r="BF2" s="31" t="s">
         <v>955</v>
       </c>
-      <c r="BG2" s="27"/>
-      <c r="BH2" s="27"/>
-      <c r="BI2" s="27"/>
-      <c r="BJ2" s="26" t="s">
+      <c r="BG2" s="32"/>
+      <c r="BH2" s="32"/>
+      <c r="BI2" s="32"/>
+      <c r="BJ2" s="31" t="s">
         <v>978</v>
       </c>
-      <c r="BK2" s="27"/>
-      <c r="BL2" s="27"/>
-      <c r="BM2" s="28"/>
+      <c r="BK2" s="32"/>
+      <c r="BL2" s="32"/>
+      <c r="BM2" s="33"/>
       <c r="BN2" s="16" t="s">
         <v>979</v>
       </c>
-      <c r="BO2" s="26" t="s">
+      <c r="BO2" s="31" t="s">
         <v>982</v>
       </c>
-      <c r="BP2" s="27"/>
-      <c r="BQ2" s="27"/>
-      <c r="BR2" s="27"/>
-      <c r="BS2" s="27"/>
-      <c r="BT2" s="28"/>
-      <c r="BU2" s="26" t="s">
+      <c r="BP2" s="32"/>
+      <c r="BQ2" s="32"/>
+      <c r="BR2" s="32"/>
+      <c r="BS2" s="32"/>
+      <c r="BT2" s="33"/>
+      <c r="BU2" s="31" t="s">
         <v>984</v>
       </c>
-      <c r="BV2" s="27"/>
-      <c r="BW2" s="28"/>
-      <c r="BX2" s="26" t="s">
+      <c r="BV2" s="32"/>
+      <c r="BW2" s="33"/>
+      <c r="BX2" s="31" t="s">
         <v>912</v>
       </c>
-      <c r="BY2" s="27"/>
-      <c r="BZ2" s="28"/>
-      <c r="CA2" s="30" t="s">
+      <c r="BY2" s="32"/>
+      <c r="BZ2" s="33"/>
+      <c r="CA2" s="28" t="s">
         <v>957</v>
       </c>
-      <c r="CB2" s="30"/>
-      <c r="CC2" s="30"/>
-      <c r="CD2" s="30"/>
+      <c r="CB2" s="28"/>
+      <c r="CC2" s="28"/>
+      <c r="CD2" s="28"/>
     </row>
     <row r="3" spans="1:82" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
@@ -15209,20 +15213,6 @@
   <sheetProtection insertColumns="0" insertRows="0" insertHyperlinks="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="23">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="CA2:CD2"/>
-    <mergeCell ref="AO2:AQ2"/>
-    <mergeCell ref="BC2:BE2"/>
-    <mergeCell ref="AR2:AX2"/>
-    <mergeCell ref="AY2:BB2"/>
-    <mergeCell ref="AR1:BE1"/>
-    <mergeCell ref="F1:AQ1"/>
-    <mergeCell ref="BJ2:BM2"/>
-    <mergeCell ref="F2:M2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="V2:AA2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="AB2:AF2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D2:E2"/>
@@ -15232,6 +15222,20 @@
     <mergeCell ref="BF2:BI2"/>
     <mergeCell ref="BO2:BT2"/>
     <mergeCell ref="BO1:BT1"/>
+    <mergeCell ref="AR1:BE1"/>
+    <mergeCell ref="F1:AQ1"/>
+    <mergeCell ref="BJ2:BM2"/>
+    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="V2:AA2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="AB2:AF2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="CA2:CD2"/>
+    <mergeCell ref="AO2:AQ2"/>
+    <mergeCell ref="BC2:BE2"/>
+    <mergeCell ref="AR2:AX2"/>
+    <mergeCell ref="AY2:BB2"/>
   </mergeCells>
   <dataValidations xWindow="491" yWindow="317" count="25">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de llenado" error="No debe de contener espacios ni caracteres especiales." promptTitle="Indicaciones" prompt="El formato debe ser XAXX010101000." sqref="J4:J104 Z4:Z104 AV4:AV104" xr:uid="{B98F17B9-63D0-482A-929E-F8CFD205118A}">
@@ -15401,7 +15405,7 @@
       <c r="D2" s="1" t="s">
         <v>922</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="24" t="s">
         <v>1008</v>
       </c>
       <c r="F2" s="1" t="s">

</xml_diff>